<commit_message>
Intermediate developement step to v0.83.16
</commit_message>
<xml_diff>
--- a/t/test_files/attr.xlsx
+++ b/t/test_files/attr.xlsx
@@ -969,13 +969,10 @@
   <dimension ref="A1:I9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
-  <cols>
-    <col min="2" max="2" width="0" hidden="1" customWidth="1"/>
-  </cols>
   <sheetData>
     <row r="1" spans="1:9">
       <c r="A1" t="s">

</xml_diff>